<commit_message>
Pork sandwich recipe set up, removed redundant function in ItemFoodBase
</commit_message>
<xml_diff>
--- a/Implementation Docs/Foods.xlsx
+++ b/Implementation Docs/Foods.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Food</t>
   </si>
@@ -425,7 +425,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,6 +487,12 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Beef sandwich recipe and advancement
</commit_message>
<xml_diff>
--- a/Implementation Docs/Foods.xlsx
+++ b/Implementation Docs/Foods.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>Food</t>
   </si>
@@ -425,7 +425,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,6 +493,9 @@
       <c r="F2" t="s">
         <v>15</v>
       </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -505,6 +508,12 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
All recipes done and tested; localization done
</commit_message>
<xml_diff>
--- a/Implementation Docs/Foods.xlsx
+++ b/Implementation Docs/Foods.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="22">
   <si>
     <t>Food</t>
   </si>
@@ -425,7 +425,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,6 +496,9 @@
       <c r="G2" t="s">
         <v>15</v>
       </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -516,6 +519,12 @@
       <c r="F3" t="s">
         <v>15</v>
       </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -530,6 +539,18 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -544,6 +565,18 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -558,6 +591,18 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -570,6 +615,18 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -586,6 +643,18 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -598,6 +667,18 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -620,6 +701,12 @@
       <c r="F10" t="s">
         <v>18</v>
       </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -639,6 +726,12 @@
       </c>
       <c r="F11" t="s">
         <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Beef and chicken sandwich sprites
</commit_message>
<xml_diff>
--- a/Implementation Docs/Foods.xlsx
+++ b/Implementation Docs/Foods.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="22">
   <si>
     <t>Food</t>
   </si>
@@ -425,7 +425,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,6 +522,9 @@
       <c r="G3" t="s">
         <v>15</v>
       </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
       <c r="I3" t="s">
         <v>15</v>
       </c>
@@ -626,7 +629,13 @@
       <c r="G7" t="s">
         <v>15</v>
       </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
       <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>